<commit_message>
Tests 01 al 66 FacturaAfecta
</commit_message>
<xml_diff>
--- a/DataPool_v2.xlsx
+++ b/DataPool_v2.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24131"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Laura Andrade\eclipse-workspace\AceptaPeru\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Verity-Usuario\eclipse-workspace\AceptaFacturasChile\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{214540D7-65E4-48AB-B646-8C1A84A37CDA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BD3F977-8BC8-4B85-9685-B217AD241D60}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20370" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1466" uniqueCount="281">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1646" uniqueCount="343">
   <si>
     <t>sebastian.acuna@verity.cl</t>
   </si>
@@ -871,6 +871,192 @@
   </si>
   <si>
     <t>103</t>
+  </si>
+  <si>
+    <t>FA_0001</t>
+  </si>
+  <si>
+    <t>13712759-8</t>
+  </si>
+  <si>
+    <t>Verity4.0</t>
+  </si>
+  <si>
+    <t>FA_0002</t>
+  </si>
+  <si>
+    <t>FA_0003</t>
+  </si>
+  <si>
+    <t>FA_0004</t>
+  </si>
+  <si>
+    <t>FA_0005</t>
+  </si>
+  <si>
+    <t>FA_0006</t>
+  </si>
+  <si>
+    <t>FA_0007</t>
+  </si>
+  <si>
+    <t>FA_0008</t>
+  </si>
+  <si>
+    <t>FA_0009</t>
+  </si>
+  <si>
+    <t>FA_0010</t>
+  </si>
+  <si>
+    <t>FA_0011</t>
+  </si>
+  <si>
+    <t>FA_0012</t>
+  </si>
+  <si>
+    <t>FA_0013</t>
+  </si>
+  <si>
+    <t>FA_0014</t>
+  </si>
+  <si>
+    <t>FA_0015</t>
+  </si>
+  <si>
+    <t>FA_0016</t>
+  </si>
+  <si>
+    <t>FA_0017</t>
+  </si>
+  <si>
+    <t>FA_0018</t>
+  </si>
+  <si>
+    <t>FA_0019</t>
+  </si>
+  <si>
+    <t>FA_0020</t>
+  </si>
+  <si>
+    <t>FA_0021</t>
+  </si>
+  <si>
+    <t>FA_0022</t>
+  </si>
+  <si>
+    <t>FA_0023</t>
+  </si>
+  <si>
+    <t>FA_0024</t>
+  </si>
+  <si>
+    <t>FA_0025</t>
+  </si>
+  <si>
+    <t>FA_0026</t>
+  </si>
+  <si>
+    <t>FA_0027</t>
+  </si>
+  <si>
+    <t>FA_0028</t>
+  </si>
+  <si>
+    <t>FA_0029</t>
+  </si>
+  <si>
+    <t>FA_0030</t>
+  </si>
+  <si>
+    <t>FA_0031</t>
+  </si>
+  <si>
+    <t>FA_0032</t>
+  </si>
+  <si>
+    <t>FA_0033</t>
+  </si>
+  <si>
+    <t>FA_0034</t>
+  </si>
+  <si>
+    <t>FA_0035</t>
+  </si>
+  <si>
+    <t>FA_0036</t>
+  </si>
+  <si>
+    <t>FA_0037</t>
+  </si>
+  <si>
+    <t>FA_0038</t>
+  </si>
+  <si>
+    <t>FA_0039</t>
+  </si>
+  <si>
+    <t>FA_0040</t>
+  </si>
+  <si>
+    <t>FA_0041</t>
+  </si>
+  <si>
+    <t>FA_0042</t>
+  </si>
+  <si>
+    <t>FA_0043</t>
+  </si>
+  <si>
+    <t>FA_0044</t>
+  </si>
+  <si>
+    <t>FA_0045</t>
+  </si>
+  <si>
+    <t>FA_0046</t>
+  </si>
+  <si>
+    <t>FA_0047</t>
+  </si>
+  <si>
+    <t>FA_0048</t>
+  </si>
+  <si>
+    <t>FA_0049</t>
+  </si>
+  <si>
+    <t>FA_0056</t>
+  </si>
+  <si>
+    <t>FA_0057</t>
+  </si>
+  <si>
+    <t>FA_0058</t>
+  </si>
+  <si>
+    <t>FA_0059</t>
+  </si>
+  <si>
+    <t>FA_0060</t>
+  </si>
+  <si>
+    <t>FA_0061</t>
+  </si>
+  <si>
+    <t>FA_0062</t>
+  </si>
+  <si>
+    <t>FA_0063</t>
+  </si>
+  <si>
+    <t>FA_0064</t>
+  </si>
+  <si>
+    <t>FA_0065</t>
+  </si>
+  <si>
+    <t>FA_0066</t>
   </si>
 </sst>
 </file>
@@ -1220,10 +1406,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:O104"/>
+  <dimension ref="A1:O164"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J87" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="M104" sqref="M101:M104"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B150" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="F161" sqref="F161"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6132,6 +6321,666 @@
       </c>
       <c r="O104" s="1" t="s">
         <v>256</v>
+      </c>
+    </row>
+    <row r="105" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A105" s="1" t="s">
+        <v>281</v>
+      </c>
+      <c r="B105" s="1" t="s">
+        <v>282</v>
+      </c>
+      <c r="C105" s="1" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="106" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A106" s="1" t="s">
+        <v>284</v>
+      </c>
+      <c r="B106" s="1" t="s">
+        <v>282</v>
+      </c>
+      <c r="C106" s="1" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="107" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A107" s="1" t="s">
+        <v>285</v>
+      </c>
+      <c r="B107" s="1" t="s">
+        <v>282</v>
+      </c>
+      <c r="C107" s="1" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="108" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A108" s="1" t="s">
+        <v>286</v>
+      </c>
+      <c r="B108" s="1" t="s">
+        <v>282</v>
+      </c>
+      <c r="C108" s="1" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="109" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A109" s="1" t="s">
+        <v>287</v>
+      </c>
+      <c r="B109" s="1" t="s">
+        <v>282</v>
+      </c>
+      <c r="C109" s="1" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="110" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A110" s="1" t="s">
+        <v>288</v>
+      </c>
+      <c r="B110" s="1" t="s">
+        <v>282</v>
+      </c>
+      <c r="C110" s="1" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="111" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A111" s="1" t="s">
+        <v>289</v>
+      </c>
+      <c r="B111" s="1" t="s">
+        <v>282</v>
+      </c>
+      <c r="C111" s="1" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="112" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A112" s="1" t="s">
+        <v>290</v>
+      </c>
+      <c r="B112" s="1" t="s">
+        <v>282</v>
+      </c>
+      <c r="C112" s="1" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="113" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A113" s="1" t="s">
+        <v>291</v>
+      </c>
+      <c r="B113" s="1" t="s">
+        <v>282</v>
+      </c>
+      <c r="C113" s="1" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="114" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A114" s="1" t="s">
+        <v>292</v>
+      </c>
+      <c r="B114" s="1" t="s">
+        <v>282</v>
+      </c>
+      <c r="C114" s="1" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="115" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A115" s="1" t="s">
+        <v>293</v>
+      </c>
+      <c r="B115" s="1" t="s">
+        <v>282</v>
+      </c>
+      <c r="C115" s="1" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="116" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A116" s="1" t="s">
+        <v>294</v>
+      </c>
+      <c r="B116" s="1" t="s">
+        <v>282</v>
+      </c>
+      <c r="C116" s="1" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="117" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A117" s="1" t="s">
+        <v>295</v>
+      </c>
+      <c r="B117" s="1" t="s">
+        <v>282</v>
+      </c>
+      <c r="C117" s="1" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="118" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A118" s="1" t="s">
+        <v>296</v>
+      </c>
+      <c r="B118" s="1" t="s">
+        <v>282</v>
+      </c>
+      <c r="C118" s="1" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="119" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A119" s="1" t="s">
+        <v>297</v>
+      </c>
+      <c r="B119" s="1" t="s">
+        <v>282</v>
+      </c>
+      <c r="C119" s="1" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="120" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A120" s="1" t="s">
+        <v>298</v>
+      </c>
+      <c r="B120" s="1" t="s">
+        <v>282</v>
+      </c>
+      <c r="C120" s="1" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="121" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A121" s="1" t="s">
+        <v>299</v>
+      </c>
+      <c r="B121" s="1" t="s">
+        <v>282</v>
+      </c>
+      <c r="C121" s="1" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="122" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A122" s="1" t="s">
+        <v>300</v>
+      </c>
+      <c r="B122" s="1" t="s">
+        <v>282</v>
+      </c>
+      <c r="C122" s="1" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="123" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A123" s="1" t="s">
+        <v>301</v>
+      </c>
+      <c r="B123" s="1" t="s">
+        <v>282</v>
+      </c>
+      <c r="C123" s="1" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="124" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A124" s="1" t="s">
+        <v>302</v>
+      </c>
+      <c r="B124" s="1" t="s">
+        <v>282</v>
+      </c>
+      <c r="C124" s="1" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="125" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A125" s="1" t="s">
+        <v>303</v>
+      </c>
+      <c r="B125" s="1" t="s">
+        <v>282</v>
+      </c>
+      <c r="C125" s="1" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="126" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A126" s="1" t="s">
+        <v>304</v>
+      </c>
+      <c r="B126" s="1" t="s">
+        <v>282</v>
+      </c>
+      <c r="C126" s="1" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="127" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A127" s="1" t="s">
+        <v>305</v>
+      </c>
+      <c r="B127" s="1" t="s">
+        <v>282</v>
+      </c>
+      <c r="C127" s="1" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="128" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A128" s="1" t="s">
+        <v>306</v>
+      </c>
+      <c r="B128" s="1" t="s">
+        <v>282</v>
+      </c>
+      <c r="C128" s="1" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="129" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A129" s="1" t="s">
+        <v>307</v>
+      </c>
+      <c r="B129" s="1" t="s">
+        <v>282</v>
+      </c>
+      <c r="C129" s="1" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="130" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A130" s="1" t="s">
+        <v>308</v>
+      </c>
+      <c r="B130" s="1" t="s">
+        <v>282</v>
+      </c>
+      <c r="C130" s="1" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="131" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A131" s="1" t="s">
+        <v>309</v>
+      </c>
+      <c r="B131" s="1" t="s">
+        <v>282</v>
+      </c>
+      <c r="C131" s="1" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="132" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A132" s="1" t="s">
+        <v>310</v>
+      </c>
+      <c r="B132" s="1" t="s">
+        <v>282</v>
+      </c>
+      <c r="C132" s="1" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="133" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A133" s="1" t="s">
+        <v>311</v>
+      </c>
+      <c r="B133" s="1" t="s">
+        <v>282</v>
+      </c>
+      <c r="C133" s="1" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="134" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A134" s="1" t="s">
+        <v>312</v>
+      </c>
+      <c r="B134" s="1" t="s">
+        <v>282</v>
+      </c>
+      <c r="C134" s="1" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="135" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A135" s="1" t="s">
+        <v>313</v>
+      </c>
+      <c r="B135" s="1" t="s">
+        <v>282</v>
+      </c>
+      <c r="C135" s="1" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="136" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A136" s="1" t="s">
+        <v>314</v>
+      </c>
+      <c r="B136" s="1" t="s">
+        <v>282</v>
+      </c>
+      <c r="C136" s="1" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="137" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A137" s="1" t="s">
+        <v>315</v>
+      </c>
+      <c r="B137" s="1" t="s">
+        <v>282</v>
+      </c>
+      <c r="C137" s="1" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="138" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A138" s="1" t="s">
+        <v>316</v>
+      </c>
+      <c r="B138" s="1" t="s">
+        <v>282</v>
+      </c>
+      <c r="C138" s="1" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="139" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A139" s="1" t="s">
+        <v>317</v>
+      </c>
+      <c r="B139" s="1" t="s">
+        <v>282</v>
+      </c>
+      <c r="C139" s="1" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="140" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A140" s="1" t="s">
+        <v>318</v>
+      </c>
+      <c r="B140" s="1" t="s">
+        <v>282</v>
+      </c>
+      <c r="C140" s="1" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="141" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A141" s="1" t="s">
+        <v>319</v>
+      </c>
+      <c r="B141" s="1" t="s">
+        <v>282</v>
+      </c>
+      <c r="C141" s="1" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="142" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A142" s="1" t="s">
+        <v>320</v>
+      </c>
+      <c r="B142" s="1" t="s">
+        <v>282</v>
+      </c>
+      <c r="C142" s="1" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="143" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A143" s="1" t="s">
+        <v>321</v>
+      </c>
+      <c r="B143" s="1" t="s">
+        <v>282</v>
+      </c>
+      <c r="C143" s="1" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="144" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A144" s="1" t="s">
+        <v>322</v>
+      </c>
+      <c r="B144" s="1" t="s">
+        <v>282</v>
+      </c>
+      <c r="C144" s="1" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="145" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A145" s="1" t="s">
+        <v>323</v>
+      </c>
+      <c r="B145" s="1" t="s">
+        <v>282</v>
+      </c>
+      <c r="C145" s="1" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="146" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A146" s="1" t="s">
+        <v>324</v>
+      </c>
+      <c r="B146" s="1" t="s">
+        <v>282</v>
+      </c>
+      <c r="C146" s="1" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="147" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A147" s="1" t="s">
+        <v>325</v>
+      </c>
+      <c r="B147" s="1" t="s">
+        <v>282</v>
+      </c>
+      <c r="C147" s="1" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="148" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A148" s="1" t="s">
+        <v>326</v>
+      </c>
+      <c r="B148" s="1" t="s">
+        <v>282</v>
+      </c>
+      <c r="C148" s="1" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="149" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A149" s="1" t="s">
+        <v>327</v>
+      </c>
+      <c r="B149" s="1" t="s">
+        <v>282</v>
+      </c>
+      <c r="C149" s="1" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="150" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A150" s="1" t="s">
+        <v>328</v>
+      </c>
+      <c r="B150" s="1" t="s">
+        <v>282</v>
+      </c>
+      <c r="C150" s="1" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="151" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A151" s="1" t="s">
+        <v>329</v>
+      </c>
+      <c r="B151" s="1" t="s">
+        <v>282</v>
+      </c>
+      <c r="C151" s="1" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="152" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A152" s="1" t="s">
+        <v>330</v>
+      </c>
+      <c r="B152" s="1" t="s">
+        <v>282</v>
+      </c>
+      <c r="C152" s="1" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="153" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A153" s="1" t="s">
+        <v>331</v>
+      </c>
+      <c r="B153" s="1" t="s">
+        <v>282</v>
+      </c>
+      <c r="C153" s="1" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="154" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A154" s="1" t="s">
+        <v>332</v>
+      </c>
+      <c r="B154" s="1" t="s">
+        <v>282</v>
+      </c>
+      <c r="C154" s="1" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="155" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A155" s="1" t="s">
+        <v>333</v>
+      </c>
+      <c r="B155" s="1" t="s">
+        <v>282</v>
+      </c>
+      <c r="C155" s="1" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="156" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A156" s="1" t="s">
+        <v>334</v>
+      </c>
+      <c r="B156" s="1" t="s">
+        <v>282</v>
+      </c>
+      <c r="C156" s="1" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="157" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A157" s="1" t="s">
+        <v>335</v>
+      </c>
+      <c r="B157" s="1" t="s">
+        <v>282</v>
+      </c>
+      <c r="C157" s="1" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="158" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A158" s="1" t="s">
+        <v>336</v>
+      </c>
+      <c r="B158" s="1" t="s">
+        <v>282</v>
+      </c>
+      <c r="C158" s="1" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="159" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A159" s="1" t="s">
+        <v>337</v>
+      </c>
+      <c r="B159" s="1" t="s">
+        <v>282</v>
+      </c>
+      <c r="C159" s="1" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="160" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A160" s="1" t="s">
+        <v>338</v>
+      </c>
+      <c r="B160" s="1" t="s">
+        <v>282</v>
+      </c>
+      <c r="C160" s="1" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="161" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A161" s="1" t="s">
+        <v>339</v>
+      </c>
+      <c r="B161" s="1" t="s">
+        <v>282</v>
+      </c>
+      <c r="C161" s="1" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="162" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A162" s="1" t="s">
+        <v>340</v>
+      </c>
+      <c r="B162" s="1" t="s">
+        <v>282</v>
+      </c>
+      <c r="C162" s="1" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="163" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A163" s="1" t="s">
+        <v>341</v>
+      </c>
+      <c r="B163" s="1" t="s">
+        <v>282</v>
+      </c>
+      <c r="C163" s="1" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="164" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A164" s="1" t="s">
+        <v>342</v>
+      </c>
+      <c r="B164" s="1" t="s">
+        <v>282</v>
+      </c>
+      <c r="C164" s="1" t="s">
+        <v>283</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Test 67 al 110 Factura Afecta y Test 01 al 35 Factura Exenta
</commit_message>
<xml_diff>
--- a/DataPool_v2.xlsx
+++ b/DataPool_v2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Verity-Usuario\eclipse-workspace\AceptaFacturasChile\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BD3F977-8BC8-4B85-9685-B217AD241D60}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C1BB0BB-AFCC-4FE7-8C55-74624ECCFD7C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1646" uniqueCount="343">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1898" uniqueCount="428">
   <si>
     <t>sebastian.acuna@verity.cl</t>
   </si>
@@ -1057,6 +1057,261 @@
   </si>
   <si>
     <t>FA_0066</t>
+  </si>
+  <si>
+    <t>18215678-7</t>
+  </si>
+  <si>
+    <t>FA_0067</t>
+  </si>
+  <si>
+    <t>FA_0068</t>
+  </si>
+  <si>
+    <t>FA_0069</t>
+  </si>
+  <si>
+    <t>FA_0070</t>
+  </si>
+  <si>
+    <t>FA_0071</t>
+  </si>
+  <si>
+    <t>FA_0072</t>
+  </si>
+  <si>
+    <t>FA_0073</t>
+  </si>
+  <si>
+    <t>FA_0074</t>
+  </si>
+  <si>
+    <t>FA_0075</t>
+  </si>
+  <si>
+    <t>FA_0076</t>
+  </si>
+  <si>
+    <t>FA_0077</t>
+  </si>
+  <si>
+    <t>FA_0078</t>
+  </si>
+  <si>
+    <t>FA_0079</t>
+  </si>
+  <si>
+    <t>FA_0080</t>
+  </si>
+  <si>
+    <t>FA_0081</t>
+  </si>
+  <si>
+    <t>FA_0082</t>
+  </si>
+  <si>
+    <t>FA_0083</t>
+  </si>
+  <si>
+    <t>FA_0084</t>
+  </si>
+  <si>
+    <t>FA_0085</t>
+  </si>
+  <si>
+    <t>FA_0086</t>
+  </si>
+  <si>
+    <t>FA_0087</t>
+  </si>
+  <si>
+    <t>FA_0088</t>
+  </si>
+  <si>
+    <t>FA_0089</t>
+  </si>
+  <si>
+    <t>FA_0090</t>
+  </si>
+  <si>
+    <t>FA_0091</t>
+  </si>
+  <si>
+    <t>FA_0092</t>
+  </si>
+  <si>
+    <t>FA_0093</t>
+  </si>
+  <si>
+    <t>FA_0094</t>
+  </si>
+  <si>
+    <t>FA_0095</t>
+  </si>
+  <si>
+    <t>FA_0096</t>
+  </si>
+  <si>
+    <t>FA_0097</t>
+  </si>
+  <si>
+    <t>FA_0098</t>
+  </si>
+  <si>
+    <t>FA_0099</t>
+  </si>
+  <si>
+    <t>FA_0100</t>
+  </si>
+  <si>
+    <t>FA_0101</t>
+  </si>
+  <si>
+    <t>FA_0102</t>
+  </si>
+  <si>
+    <t>FA_0103</t>
+  </si>
+  <si>
+    <t>FA_0104</t>
+  </si>
+  <si>
+    <t>FA_0105</t>
+  </si>
+  <si>
+    <t>FA_0106</t>
+  </si>
+  <si>
+    <t>FA_0107</t>
+  </si>
+  <si>
+    <t>FA_0108</t>
+  </si>
+  <si>
+    <t>FA_0109</t>
+  </si>
+  <si>
+    <t>FA_0110</t>
+  </si>
+  <si>
+    <t>FE_0001</t>
+  </si>
+  <si>
+    <t>FE_0002</t>
+  </si>
+  <si>
+    <t>FE_0003</t>
+  </si>
+  <si>
+    <t>FE_0004</t>
+  </si>
+  <si>
+    <t>FE_0005</t>
+  </si>
+  <si>
+    <t>FE_0006</t>
+  </si>
+  <si>
+    <t>FE_0007</t>
+  </si>
+  <si>
+    <t>FE_0008</t>
+  </si>
+  <si>
+    <t>FE_0009</t>
+  </si>
+  <si>
+    <t>FE_0010</t>
+  </si>
+  <si>
+    <t>FE_0011</t>
+  </si>
+  <si>
+    <t>FE_0012</t>
+  </si>
+  <si>
+    <t>FE_0013</t>
+  </si>
+  <si>
+    <t>FE_0014</t>
+  </si>
+  <si>
+    <t>FE_0015</t>
+  </si>
+  <si>
+    <t>FE_0016</t>
+  </si>
+  <si>
+    <t>FE_0017</t>
+  </si>
+  <si>
+    <t>FE_0018</t>
+  </si>
+  <si>
+    <t>FE_0019</t>
+  </si>
+  <si>
+    <t>FE_0020</t>
+  </si>
+  <si>
+    <t>FE_0021</t>
+  </si>
+  <si>
+    <t>FE_0022</t>
+  </si>
+  <si>
+    <t>FE_0023</t>
+  </si>
+  <si>
+    <t>FE_0024</t>
+  </si>
+  <si>
+    <t>FE_0025</t>
+  </si>
+  <si>
+    <t>FE_0026</t>
+  </si>
+  <si>
+    <t>FE_0027</t>
+  </si>
+  <si>
+    <t>FE_0028</t>
+  </si>
+  <si>
+    <t>FE_0029</t>
+  </si>
+  <si>
+    <t>FE_0030</t>
+  </si>
+  <si>
+    <t>FE_0031</t>
+  </si>
+  <si>
+    <t>FE_0032</t>
+  </si>
+  <si>
+    <t>FE_0033</t>
+  </si>
+  <si>
+    <t>FE_0034</t>
+  </si>
+  <si>
+    <t>FE_0035</t>
+  </si>
+  <si>
+    <t>FE_0036</t>
+  </si>
+  <si>
+    <t>FE_0037</t>
+  </si>
+  <si>
+    <t>FE_0038</t>
+  </si>
+  <si>
+    <t>FE_0039</t>
+  </si>
+  <si>
+    <t>FE_0040</t>
   </si>
 </sst>
 </file>
@@ -1406,13 +1661,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:O164"/>
+  <dimension ref="A1:O248"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B150" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B237" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F161" sqref="F161"/>
+      <selection pane="bottomRight" activeCell="E246" sqref="E246"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6977,9 +7232,933 @@
         <v>342</v>
       </c>
       <c r="B164" s="1" t="s">
-        <v>282</v>
+        <v>343</v>
       </c>
       <c r="C164" s="1" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="165" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A165" s="1" t="s">
+        <v>344</v>
+      </c>
+      <c r="B165" s="1" t="s">
+        <v>343</v>
+      </c>
+      <c r="C165" s="1" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="166" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A166" s="1" t="s">
+        <v>345</v>
+      </c>
+      <c r="B166" s="1" t="s">
+        <v>343</v>
+      </c>
+      <c r="C166" s="1" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="167" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A167" s="1" t="s">
+        <v>346</v>
+      </c>
+      <c r="B167" s="1" t="s">
+        <v>343</v>
+      </c>
+      <c r="C167" s="1" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="168" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A168" s="1" t="s">
+        <v>347</v>
+      </c>
+      <c r="B168" s="1" t="s">
+        <v>343</v>
+      </c>
+      <c r="C168" s="1" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="169" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A169" s="1" t="s">
+        <v>348</v>
+      </c>
+      <c r="B169" s="1" t="s">
+        <v>343</v>
+      </c>
+      <c r="C169" s="1" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="170" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A170" s="1" t="s">
+        <v>349</v>
+      </c>
+      <c r="B170" s="1" t="s">
+        <v>343</v>
+      </c>
+      <c r="C170" s="1" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="171" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A171" s="1" t="s">
+        <v>350</v>
+      </c>
+      <c r="B171" s="1" t="s">
+        <v>343</v>
+      </c>
+      <c r="C171" s="1" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="172" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A172" s="1" t="s">
+        <v>351</v>
+      </c>
+      <c r="B172" s="1" t="s">
+        <v>343</v>
+      </c>
+      <c r="C172" s="1" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="173" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A173" s="1" t="s">
+        <v>352</v>
+      </c>
+      <c r="B173" s="1" t="s">
+        <v>343</v>
+      </c>
+      <c r="C173" s="1" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="174" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A174" s="1" t="s">
+        <v>353</v>
+      </c>
+      <c r="B174" s="1" t="s">
+        <v>343</v>
+      </c>
+      <c r="C174" s="1" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="175" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A175" s="1" t="s">
+        <v>354</v>
+      </c>
+      <c r="B175" s="1" t="s">
+        <v>343</v>
+      </c>
+      <c r="C175" s="1" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="176" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A176" s="1" t="s">
+        <v>355</v>
+      </c>
+      <c r="B176" s="1" t="s">
+        <v>343</v>
+      </c>
+      <c r="C176" s="1" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="177" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A177" s="1" t="s">
+        <v>356</v>
+      </c>
+      <c r="B177" s="1" t="s">
+        <v>343</v>
+      </c>
+      <c r="C177" s="1" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="178" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A178" s="1" t="s">
+        <v>357</v>
+      </c>
+      <c r="B178" s="1" t="s">
+        <v>343</v>
+      </c>
+      <c r="C178" s="1" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="179" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A179" s="1" t="s">
+        <v>358</v>
+      </c>
+      <c r="B179" s="1" t="s">
+        <v>343</v>
+      </c>
+      <c r="C179" s="1" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="180" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A180" s="1" t="s">
+        <v>359</v>
+      </c>
+      <c r="B180" s="1" t="s">
+        <v>343</v>
+      </c>
+      <c r="C180" s="1" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="181" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A181" s="1" t="s">
+        <v>360</v>
+      </c>
+      <c r="B181" s="1" t="s">
+        <v>343</v>
+      </c>
+      <c r="C181" s="1" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="182" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A182" s="1" t="s">
+        <v>361</v>
+      </c>
+      <c r="B182" s="1" t="s">
+        <v>343</v>
+      </c>
+      <c r="C182" s="1" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="183" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A183" s="1" t="s">
+        <v>362</v>
+      </c>
+      <c r="B183" s="1" t="s">
+        <v>343</v>
+      </c>
+      <c r="C183" s="1" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="184" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A184" s="1" t="s">
+        <v>363</v>
+      </c>
+      <c r="B184" s="1" t="s">
+        <v>343</v>
+      </c>
+      <c r="C184" s="1" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="185" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A185" s="1" t="s">
+        <v>364</v>
+      </c>
+      <c r="B185" s="1" t="s">
+        <v>343</v>
+      </c>
+      <c r="C185" s="1" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="186" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A186" s="1" t="s">
+        <v>365</v>
+      </c>
+      <c r="B186" s="1" t="s">
+        <v>343</v>
+      </c>
+      <c r="C186" s="1" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="187" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A187" s="1" t="s">
+        <v>366</v>
+      </c>
+      <c r="B187" s="1" t="s">
+        <v>343</v>
+      </c>
+      <c r="C187" s="1" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="188" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A188" s="1" t="s">
+        <v>367</v>
+      </c>
+      <c r="B188" s="1" t="s">
+        <v>343</v>
+      </c>
+      <c r="C188" s="1" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="189" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A189" s="1" t="s">
+        <v>368</v>
+      </c>
+      <c r="B189" s="1" t="s">
+        <v>343</v>
+      </c>
+      <c r="C189" s="1" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="190" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A190" s="1" t="s">
+        <v>369</v>
+      </c>
+      <c r="B190" s="1" t="s">
+        <v>343</v>
+      </c>
+      <c r="C190" s="1" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="191" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A191" s="1" t="s">
+        <v>370</v>
+      </c>
+      <c r="B191" s="1" t="s">
+        <v>343</v>
+      </c>
+      <c r="C191" s="1" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="192" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A192" s="1" t="s">
+        <v>371</v>
+      </c>
+      <c r="B192" s="1" t="s">
+        <v>343</v>
+      </c>
+      <c r="C192" s="1" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="193" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A193" s="1" t="s">
+        <v>372</v>
+      </c>
+      <c r="B193" s="1" t="s">
+        <v>343</v>
+      </c>
+      <c r="C193" s="1" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="194" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A194" s="1" t="s">
+        <v>373</v>
+      </c>
+      <c r="B194" s="1" t="s">
+        <v>343</v>
+      </c>
+      <c r="C194" s="1" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="195" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A195" s="1" t="s">
+        <v>374</v>
+      </c>
+      <c r="B195" s="1" t="s">
+        <v>343</v>
+      </c>
+      <c r="C195" s="1" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="196" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A196" s="1" t="s">
+        <v>375</v>
+      </c>
+      <c r="B196" s="1" t="s">
+        <v>343</v>
+      </c>
+      <c r="C196" s="1" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="197" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A197" s="1" t="s">
+        <v>376</v>
+      </c>
+      <c r="B197" s="1" t="s">
+        <v>343</v>
+      </c>
+      <c r="C197" s="1" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="198" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A198" s="1" t="s">
+        <v>377</v>
+      </c>
+      <c r="B198" s="1" t="s">
+        <v>343</v>
+      </c>
+      <c r="C198" s="1" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="199" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A199" s="1" t="s">
+        <v>378</v>
+      </c>
+      <c r="B199" s="1" t="s">
+        <v>343</v>
+      </c>
+      <c r="C199" s="1" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="200" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A200" s="1" t="s">
+        <v>379</v>
+      </c>
+      <c r="B200" s="1" t="s">
+        <v>343</v>
+      </c>
+      <c r="C200" s="1" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="201" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A201" s="1" t="s">
+        <v>380</v>
+      </c>
+      <c r="B201" s="1" t="s">
+        <v>343</v>
+      </c>
+      <c r="C201" s="1" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="202" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A202" s="1" t="s">
+        <v>381</v>
+      </c>
+      <c r="B202" s="1" t="s">
+        <v>343</v>
+      </c>
+      <c r="C202" s="1" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="203" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A203" s="1" t="s">
+        <v>382</v>
+      </c>
+      <c r="B203" s="1" t="s">
+        <v>343</v>
+      </c>
+      <c r="C203" s="1" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="204" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A204" s="1" t="s">
+        <v>383</v>
+      </c>
+      <c r="B204" s="1" t="s">
+        <v>343</v>
+      </c>
+      <c r="C204" s="1" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="205" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A205" s="1" t="s">
+        <v>384</v>
+      </c>
+      <c r="B205" s="1" t="s">
+        <v>343</v>
+      </c>
+      <c r="C205" s="1" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="206" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A206" s="1" t="s">
+        <v>385</v>
+      </c>
+      <c r="B206" s="1" t="s">
+        <v>343</v>
+      </c>
+      <c r="C206" s="1" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="207" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A207" s="1" t="s">
+        <v>386</v>
+      </c>
+      <c r="B207" s="1" t="s">
+        <v>343</v>
+      </c>
+      <c r="C207" s="1" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="208" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A208" s="1" t="s">
+        <v>387</v>
+      </c>
+      <c r="B208" s="1" t="s">
+        <v>343</v>
+      </c>
+      <c r="C208" s="1" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="209" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A209" s="1" t="s">
+        <v>388</v>
+      </c>
+      <c r="B209" s="1" t="s">
+        <v>343</v>
+      </c>
+      <c r="C209" s="1" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="210" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A210" s="1" t="s">
+        <v>389</v>
+      </c>
+      <c r="B210" s="1" t="s">
+        <v>343</v>
+      </c>
+      <c r="C210" s="1" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="211" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A211" s="1" t="s">
+        <v>390</v>
+      </c>
+      <c r="B211" s="1" t="s">
+        <v>343</v>
+      </c>
+      <c r="C211" s="1" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="212" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A212" s="1" t="s">
+        <v>391</v>
+      </c>
+      <c r="B212" s="1" t="s">
+        <v>343</v>
+      </c>
+      <c r="C212" s="1" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="213" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A213" s="1" t="s">
+        <v>392</v>
+      </c>
+      <c r="B213" s="1" t="s">
+        <v>343</v>
+      </c>
+      <c r="C213" s="1" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="214" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A214" s="1" t="s">
+        <v>393</v>
+      </c>
+      <c r="B214" s="1" t="s">
+        <v>343</v>
+      </c>
+      <c r="C214" s="1" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="215" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A215" s="1" t="s">
+        <v>394</v>
+      </c>
+      <c r="B215" s="1" t="s">
+        <v>343</v>
+      </c>
+      <c r="C215" s="1" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="216" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A216" s="1" t="s">
+        <v>395</v>
+      </c>
+      <c r="B216" s="1" t="s">
+        <v>343</v>
+      </c>
+      <c r="C216" s="1" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="217" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A217" s="1" t="s">
+        <v>396</v>
+      </c>
+      <c r="B217" s="1" t="s">
+        <v>343</v>
+      </c>
+      <c r="C217" s="1" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="218" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A218" s="1" t="s">
+        <v>397</v>
+      </c>
+      <c r="B218" s="1" t="s">
+        <v>343</v>
+      </c>
+      <c r="C218" s="1" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="219" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A219" s="1" t="s">
+        <v>398</v>
+      </c>
+      <c r="B219" s="1" t="s">
+        <v>343</v>
+      </c>
+      <c r="C219" s="1" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="220" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A220" s="1" t="s">
+        <v>399</v>
+      </c>
+      <c r="B220" s="1" t="s">
+        <v>343</v>
+      </c>
+      <c r="C220" s="1" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="221" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A221" s="1" t="s">
+        <v>400</v>
+      </c>
+      <c r="B221" s="1" t="s">
+        <v>343</v>
+      </c>
+      <c r="C221" s="1" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="222" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A222" s="1" t="s">
+        <v>401</v>
+      </c>
+      <c r="B222" s="1" t="s">
+        <v>343</v>
+      </c>
+      <c r="C222" s="1" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="223" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A223" s="1" t="s">
+        <v>402</v>
+      </c>
+      <c r="B223" s="1" t="s">
+        <v>343</v>
+      </c>
+      <c r="C223" s="1" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="224" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A224" s="1" t="s">
+        <v>403</v>
+      </c>
+      <c r="B224" s="1" t="s">
+        <v>343</v>
+      </c>
+      <c r="C224" s="1" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="225" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A225" s="1" t="s">
+        <v>404</v>
+      </c>
+      <c r="B225" s="1" t="s">
+        <v>343</v>
+      </c>
+      <c r="C225" s="1" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="226" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A226" s="1" t="s">
+        <v>405</v>
+      </c>
+      <c r="B226" s="1" t="s">
+        <v>343</v>
+      </c>
+      <c r="C226" s="1" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="227" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A227" s="1" t="s">
+        <v>406</v>
+      </c>
+      <c r="B227" s="1" t="s">
+        <v>343</v>
+      </c>
+      <c r="C227" s="1" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="228" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A228" s="1" t="s">
+        <v>407</v>
+      </c>
+      <c r="B228" s="1" t="s">
+        <v>343</v>
+      </c>
+      <c r="C228" s="1" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="229" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A229" s="1" t="s">
+        <v>408</v>
+      </c>
+      <c r="B229" s="1" t="s">
+        <v>343</v>
+      </c>
+      <c r="C229" s="1" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="230" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A230" s="1" t="s">
+        <v>409</v>
+      </c>
+      <c r="B230" s="1" t="s">
+        <v>343</v>
+      </c>
+      <c r="C230" s="1" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="231" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A231" s="1" t="s">
+        <v>410</v>
+      </c>
+      <c r="B231" s="1" t="s">
+        <v>343</v>
+      </c>
+      <c r="C231" s="1" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="232" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A232" s="1" t="s">
+        <v>411</v>
+      </c>
+      <c r="B232" s="1" t="s">
+        <v>343</v>
+      </c>
+      <c r="C232" s="1" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="233" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A233" s="1" t="s">
+        <v>412</v>
+      </c>
+      <c r="B233" s="1" t="s">
+        <v>343</v>
+      </c>
+      <c r="C233" s="1" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="234" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A234" s="1" t="s">
+        <v>413</v>
+      </c>
+      <c r="B234" s="1" t="s">
+        <v>343</v>
+      </c>
+      <c r="C234" s="1" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="235" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A235" s="1" t="s">
+        <v>414</v>
+      </c>
+      <c r="B235" s="1" t="s">
+        <v>343</v>
+      </c>
+      <c r="C235" s="1" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="236" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A236" s="1" t="s">
+        <v>415</v>
+      </c>
+      <c r="B236" s="1" t="s">
+        <v>343</v>
+      </c>
+      <c r="C236" s="1" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="237" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A237" s="1" t="s">
+        <v>416</v>
+      </c>
+      <c r="B237" s="1" t="s">
+        <v>343</v>
+      </c>
+      <c r="C237" s="1" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="238" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A238" s="1" t="s">
+        <v>417</v>
+      </c>
+      <c r="B238" s="1" t="s">
+        <v>343</v>
+      </c>
+      <c r="C238" s="1" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="239" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A239" s="1" t="s">
+        <v>418</v>
+      </c>
+      <c r="B239" s="1" t="s">
+        <v>343</v>
+      </c>
+      <c r="C239" s="1" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="240" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A240" s="1" t="s">
+        <v>419</v>
+      </c>
+      <c r="B240" s="1" t="s">
+        <v>343</v>
+      </c>
+      <c r="C240" s="1" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="241" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A241" s="1" t="s">
+        <v>420</v>
+      </c>
+      <c r="B241" s="1" t="s">
+        <v>343</v>
+      </c>
+      <c r="C241" s="1" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="242" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A242" s="1" t="s">
+        <v>421</v>
+      </c>
+      <c r="B242" s="1" t="s">
+        <v>343</v>
+      </c>
+      <c r="C242" s="1" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="243" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A243" s="1" t="s">
+        <v>422</v>
+      </c>
+      <c r="B243" s="1" t="s">
+        <v>343</v>
+      </c>
+      <c r="C243" s="1" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="244" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A244" s="1" t="s">
+        <v>423</v>
+      </c>
+      <c r="B244" s="1" t="s">
+        <v>343</v>
+      </c>
+      <c r="C244" s="1" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="245" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A245" s="1" t="s">
+        <v>424</v>
+      </c>
+      <c r="B245" s="1" t="s">
+        <v>343</v>
+      </c>
+      <c r="C245" s="1" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="246" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A246" s="1" t="s">
+        <v>425</v>
+      </c>
+      <c r="B246" s="1" t="s">
+        <v>343</v>
+      </c>
+      <c r="C246" s="1" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="247" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A247" s="1" t="s">
+        <v>426</v>
+      </c>
+      <c r="B247" s="1" t="s">
+        <v>343</v>
+      </c>
+      <c r="C247" s="1" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="248" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A248" s="1" t="s">
+        <v>427</v>
+      </c>
+      <c r="B248" s="1" t="s">
+        <v>343</v>
+      </c>
+      <c r="C248" s="1" t="s">
         <v>283</v>
       </c>
     </row>

</xml_diff>